<commit_message>
subida entrega numero 1, lab 1-3
</commit_message>
<xml_diff>
--- a/algstudent/comparativa_lab1_2.xlsx
+++ b/algstudent/comparativa_lab1_2.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmene\Documents\2o\Algoritmia\algorithmics-template\algstudent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD3F7408-959E-4DE1-BE22-4F75340DBB11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3280E902-4BAB-4EDB-967F-6DCC4563AEC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lab 1" sheetId="1" r:id="rId1"/>
     <sheet name="Lab 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Lab3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="68">
   <si>
     <t>Executions</t>
   </si>
@@ -169,6 +171,78 @@
   </si>
   <si>
     <t>(OOT)109634</t>
+  </si>
+  <si>
+    <t>tLoop1</t>
+  </si>
+  <si>
+    <t>tLoop3</t>
+  </si>
+  <si>
+    <t>tLoop2</t>
+  </si>
+  <si>
+    <t>repetitions</t>
+  </si>
+  <si>
+    <t>(OOT)164291</t>
+  </si>
+  <si>
+    <t>tLoop4</t>
+  </si>
+  <si>
+    <t>(OOT)83004</t>
+  </si>
+  <si>
+    <t>tLoop5</t>
+  </si>
+  <si>
+    <t>tLoop6</t>
+  </si>
+  <si>
+    <t>tLoop7</t>
+  </si>
+  <si>
+    <t>(OOT)77063</t>
+  </si>
+  <si>
+    <t>t1/t2</t>
+  </si>
+  <si>
+    <t>t3/t2</t>
+  </si>
+  <si>
+    <t>tLoop4(PY)-t41</t>
+  </si>
+  <si>
+    <t>tLoop4(Java No OP)-t42</t>
+  </si>
+  <si>
+    <t>tLoop4(Java OP)-t43</t>
+  </si>
+  <si>
+    <t>t43/t42</t>
+  </si>
+  <si>
+    <t>t42/t41</t>
+  </si>
+  <si>
+    <t>(OOT)7706300</t>
+  </si>
+  <si>
+    <t>(OOT)1467900</t>
+  </si>
+  <si>
+    <t>(OOT)243300</t>
+  </si>
+  <si>
+    <t>(OOT)25300</t>
+  </si>
+  <si>
+    <t>(OOT)57300</t>
+  </si>
+  <si>
+    <t>(OOT)674700</t>
   </si>
 </sst>
 </file>
@@ -192,7 +266,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -226,6 +300,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -338,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -364,9 +450,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -381,7 +464,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -410,6 +493,34 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -692,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -720,13 +831,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="24">
+      <c r="A2" s="23">
         <v>10000</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="26">
         <v>2608</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="26">
         <v>23</v>
       </c>
       <c r="H2" s="5" t="s">
@@ -740,13 +851,13 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="24">
+      <c r="A3" s="23">
         <v>20000</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="27">
         <v>10866</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="27">
         <v>73</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -760,13 +871,13 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="24">
+      <c r="A4" s="23">
         <v>40000</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="27">
         <v>44849</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="27">
         <v>245</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -780,13 +891,13 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="24">
+      <c r="A5" s="23">
         <v>80000</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="27">
         <v>965</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -794,35 +905,35 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="24">
+      <c r="A6" s="23">
         <v>16000</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="27">
         <v>3623</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="24">
+      <c r="A7" s="23">
         <v>320000</v>
       </c>
-      <c r="B7" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="B7" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="27">
         <v>13545</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="24">
+      <c r="A8" s="23">
         <v>640000</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B8" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="27">
         <v>49692</v>
       </c>
     </row>
@@ -830,10 +941,10 @@
       <c r="A9" s="5">
         <v>128000</v>
       </c>
-      <c r="B9" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="40" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="4"/>
@@ -877,7 +988,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="20">
+      <c r="A13" s="19">
         <v>10000</v>
       </c>
       <c r="B13" s="12">
@@ -909,7 +1020,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="20">
+      <c r="A14" s="19">
         <v>20000</v>
       </c>
       <c r="B14" s="10">
@@ -941,7 +1052,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="20">
+      <c r="A15" s="19">
         <v>40000</v>
       </c>
       <c r="B15" s="10">
@@ -973,7 +1084,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="20">
+      <c r="A16" s="19">
         <v>80000</v>
       </c>
       <c r="B16" s="10" t="s">
@@ -1004,17 +1115,17 @@
         <v>3389</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="20">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A17" s="19">
         <v>16000</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="20" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="10">
         <v>31797</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="D17" s="22" t="s">
         <v>23</v>
       </c>
       <c r="E17" s="10">
@@ -1036,17 +1147,17 @@
         <v>11567</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="20">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A18" s="19">
         <v>320000</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="20" t="s">
         <v>2</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="D18" s="20" t="s">
         <v>2</v>
       </c>
       <c r="E18" s="17" t="s">
@@ -1068,17 +1179,17 @@
         <v>37217</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="20">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A19" s="19">
         <v>640000</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="20" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="20" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="14" t="s">
@@ -1100,17 +1211,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="11">
         <v>128000</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="21" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="21" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="15" t="s">
@@ -1128,7 +1239,349 @@
       <c r="I20" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="J20" s="15"/>
+      <c r="J20" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A23" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="L23" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="M23" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="N23" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="O23" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A24" s="19">
+        <v>10000</v>
+      </c>
+      <c r="B24" s="12">
+        <v>2545</v>
+      </c>
+      <c r="C24" s="12">
+        <v>300</v>
+      </c>
+      <c r="D24" s="12">
+        <v>136</v>
+      </c>
+      <c r="G24" s="19">
+        <v>10000</v>
+      </c>
+      <c r="H24" s="12">
+        <v>717</v>
+      </c>
+      <c r="I24" s="12">
+        <v>96</v>
+      </c>
+      <c r="J24" s="12">
+        <v>60</v>
+      </c>
+      <c r="L24" s="19">
+        <v>10000</v>
+      </c>
+      <c r="M24" s="12">
+        <v>121</v>
+      </c>
+      <c r="N24" s="12">
+        <v>17</v>
+      </c>
+      <c r="O24" s="12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A25" s="19">
+        <v>20000</v>
+      </c>
+      <c r="B25" s="10">
+        <v>9277</v>
+      </c>
+      <c r="C25" s="10">
+        <v>1101</v>
+      </c>
+      <c r="D25" s="10">
+        <v>541</v>
+      </c>
+      <c r="G25" s="19">
+        <v>20000</v>
+      </c>
+      <c r="H25" s="10">
+        <v>3461</v>
+      </c>
+      <c r="I25" s="10">
+        <v>420</v>
+      </c>
+      <c r="J25" s="10">
+        <v>296</v>
+      </c>
+      <c r="L25" s="19">
+        <v>20000</v>
+      </c>
+      <c r="M25" s="10">
+        <v>621</v>
+      </c>
+      <c r="N25" s="10">
+        <v>102</v>
+      </c>
+      <c r="O25" s="10">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A26" s="19">
+        <v>40000</v>
+      </c>
+      <c r="B26" s="10">
+        <v>31475</v>
+      </c>
+      <c r="C26" s="10">
+        <v>3514</v>
+      </c>
+      <c r="D26" s="10">
+        <v>2060</v>
+      </c>
+      <c r="G26" s="19">
+        <v>40000</v>
+      </c>
+      <c r="H26" s="10">
+        <v>12497</v>
+      </c>
+      <c r="I26" s="10">
+        <v>1537</v>
+      </c>
+      <c r="J26" s="10">
+        <v>951</v>
+      </c>
+      <c r="L26" s="19">
+        <v>40000</v>
+      </c>
+      <c r="M26" s="10">
+        <v>2483</v>
+      </c>
+      <c r="N26" s="10">
+        <v>288</v>
+      </c>
+      <c r="O26" s="10">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A27" s="19">
+        <v>80000</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="10">
+        <v>12378</v>
+      </c>
+      <c r="D27" s="10">
+        <v>6943</v>
+      </c>
+      <c r="G27" s="19">
+        <v>80000</v>
+      </c>
+      <c r="H27" s="10">
+        <v>43676</v>
+      </c>
+      <c r="I27" s="10">
+        <v>5361</v>
+      </c>
+      <c r="J27" s="10">
+        <v>3389</v>
+      </c>
+      <c r="L27" s="19">
+        <v>80000</v>
+      </c>
+      <c r="M27" s="10">
+        <v>9453</v>
+      </c>
+      <c r="N27" s="10">
+        <v>981</v>
+      </c>
+      <c r="O27" s="10">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A28" s="19">
+        <v>16000</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="10">
+        <v>44967</v>
+      </c>
+      <c r="D28" s="10">
+        <v>21624</v>
+      </c>
+      <c r="G28" s="19">
+        <v>16000</v>
+      </c>
+      <c r="H28" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="I28" s="10">
+        <v>17147</v>
+      </c>
+      <c r="J28" s="10">
+        <v>11567</v>
+      </c>
+      <c r="L28" s="19">
+        <v>16000</v>
+      </c>
+      <c r="M28" s="10">
+        <v>31797</v>
+      </c>
+      <c r="N28" s="10">
+        <v>3586</v>
+      </c>
+      <c r="O28" s="10">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A29" s="19">
+        <v>320000</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" s="19">
+        <v>320000</v>
+      </c>
+      <c r="H29" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="I29" s="10">
+        <v>57761</v>
+      </c>
+      <c r="J29" s="10">
+        <v>37217</v>
+      </c>
+      <c r="L29" s="19">
+        <v>320000</v>
+      </c>
+      <c r="M29" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N29" s="10">
+        <v>12107</v>
+      </c>
+      <c r="O29" s="10">
+        <v>6779</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A30" s="19">
+        <v>640000</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" s="19">
+        <v>640000</v>
+      </c>
+      <c r="H30" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="I30" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="J30" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="L30" s="19">
+        <v>640000</v>
+      </c>
+      <c r="M30" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="N30" s="10">
+        <v>40205</v>
+      </c>
+      <c r="O30" s="10">
+        <v>21252</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A31" s="11">
+        <v>128000</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G31" s="11">
+        <v>128000</v>
+      </c>
+      <c r="H31" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="I31" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J31" s="15"/>
+      <c r="L31" s="11">
+        <v>128000</v>
+      </c>
+      <c r="M31" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="N31" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="O31" s="13" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1138,10 +1591,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77251859-197B-43E1-9899-81A4CD096836}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1151,22 +1604,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="35" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1174,20 +1627,20 @@
       <c r="A2" s="3">
         <v>100000</v>
       </c>
-      <c r="B2" s="27">
+      <c r="B2" s="26">
         <v>151</v>
       </c>
-      <c r="C2" s="27">
+      <c r="C2" s="26">
         <v>154</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="31">
         <v>710</v>
       </c>
-      <c r="E2" s="35" t="str">
+      <c r="E2" s="34" t="str">
         <f>"(OOT)" &amp; D2 * E$17</f>
         <v>(OOT)710000</v>
       </c>
-      <c r="F2" s="27">
+      <c r="F2" s="26">
         <v>238</v>
       </c>
     </row>
@@ -1195,20 +1648,20 @@
       <c r="A3" s="3">
         <v>200000</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="27">
         <v>297</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="27">
         <v>310</v>
       </c>
-      <c r="D3" s="31">
+      <c r="D3" s="30">
         <v>2951</v>
       </c>
-      <c r="E3" s="37" t="str">
+      <c r="E3" s="36" t="str">
         <f t="shared" ref="E3:E5" si="0">"(OOT)" &amp; D3 * E$17</f>
         <v>(OOT)2951000</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F3" s="27">
         <v>382</v>
       </c>
       <c r="J3" s="5" t="s">
@@ -1222,20 +1675,20 @@
       <c r="A4" s="3">
         <v>400000</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="27">
         <v>695</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4" s="27">
         <v>592</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="30">
         <v>11933</v>
       </c>
-      <c r="E4" s="37" t="str">
+      <c r="E4" s="36" t="str">
         <f t="shared" si="0"/>
         <v>(OOT)11933000</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="27">
         <v>818</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -1249,20 +1702,20 @@
       <c r="A5" s="3">
         <v>800000</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="27">
         <v>1276</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="27">
         <v>1264</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="30">
         <v>47397</v>
       </c>
-      <c r="E5" s="37" t="str">
+      <c r="E5" s="36" t="str">
         <f t="shared" si="0"/>
         <v>(OOT)47397000</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="27">
         <v>1623</v>
       </c>
       <c r="J5" s="1" t="s">
@@ -1276,19 +1729,19 @@
       <c r="A6" s="3">
         <v>1600000</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="27">
         <v>2115</v>
       </c>
-      <c r="C6" s="28">
+      <c r="C6" s="27">
         <v>2425</v>
       </c>
-      <c r="D6" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="28">
+      <c r="D6" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="27">
         <v>3101</v>
       </c>
     </row>
@@ -1296,19 +1749,19 @@
       <c r="A7" s="3">
         <v>3200000</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="27">
         <v>3767</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="27">
         <v>4648</v>
       </c>
-      <c r="D7" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="28">
+      <c r="D7" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="27">
         <v>6548</v>
       </c>
     </row>
@@ -1316,19 +1769,19 @@
       <c r="A8" s="3">
         <v>6400000</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="27">
         <v>7393</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="27">
         <v>9177</v>
       </c>
-      <c r="D8" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="28">
+      <c r="D8" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="27">
         <v>13033</v>
       </c>
     </row>
@@ -1336,19 +1789,19 @@
       <c r="A9" s="3">
         <v>1280000</v>
       </c>
-      <c r="B9" s="28">
+      <c r="B9" s="27">
         <v>14062</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="27">
         <v>17509</v>
       </c>
-      <c r="D9" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="28">
+      <c r="D9" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="27">
         <v>25296</v>
       </c>
     </row>
@@ -1356,19 +1809,19 @@
       <c r="A10" s="3">
         <v>2560000</v>
       </c>
-      <c r="B10" s="28">
+      <c r="B10" s="27">
         <v>27054</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10" s="27">
         <v>32829</v>
       </c>
-      <c r="D10" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="28">
+      <c r="D10" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="27">
         <v>53244</v>
       </c>
     </row>
@@ -1376,19 +1829,19 @@
       <c r="A11" s="3">
         <v>5120000</v>
       </c>
-      <c r="B11" s="28">
+      <c r="B11" s="27">
         <v>50658</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="28" t="s">
+      <c r="D11" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="27" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1396,83 +1849,134 @@
       <c r="A12" s="3">
         <v>10240000</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="29" t="s">
-        <v>2</v>
+      <c r="C12" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="K12" s="35" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>20480000</v>
       </c>
-      <c r="B13" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="29" t="s">
-        <v>2</v>
+      <c r="B13" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="I13" s="3">
+        <v>100000</v>
+      </c>
+      <c r="J13" s="34" t="e">
+        <f>"(OOT)" &amp; I13 * J$17</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K13" s="26">
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>40960000</v>
       </c>
-      <c r="B14" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="29" t="s">
-        <v>2</v>
+      <c r="B14" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="3">
+        <v>200000</v>
+      </c>
+      <c r="J14" s="36" t="e">
+        <f t="shared" ref="J14:J16" si="1">"(OOT)" &amp; I14 * J$17</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K14" s="27">
+        <v>382</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>81920000</v>
       </c>
-      <c r="B15" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="30" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B15" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="I15" s="3">
+        <v>400000</v>
+      </c>
+      <c r="J15" s="36" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K15" s="27">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I16" s="3">
+        <v>800000</v>
+      </c>
+      <c r="J16" s="36" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K16" s="27">
+        <v>1623</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1488,10 +1992,1262 @@
       <c r="E17">
         <v>1000</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E18" s="26" t="s">
+      <c r="I17" s="3">
+        <v>1600000</v>
+      </c>
+      <c r="J17" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="K17" s="27">
+        <v>3101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="E18" s="25" t="s">
         <v>40</v>
+      </c>
+      <c r="I18" s="3">
+        <v>3200000</v>
+      </c>
+      <c r="J18" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="K18" s="27">
+        <v>6548</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I19" s="3">
+        <v>6400000</v>
+      </c>
+      <c r="J19" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" s="27">
+        <v>13033</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I20" s="3">
+        <v>1280000</v>
+      </c>
+      <c r="J20" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="K20" s="27">
+        <v>25296</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I21" s="3">
+        <v>2560000</v>
+      </c>
+      <c r="J21" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="K21" s="27">
+        <v>53244</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I22" s="3">
+        <v>5120000</v>
+      </c>
+      <c r="J22" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="K22" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I23" s="3">
+        <v>10240000</v>
+      </c>
+      <c r="J23" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="K23" s="28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I24" s="3">
+        <v>20480000</v>
+      </c>
+      <c r="J24" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="K24" s="28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I25" s="3">
+        <v>40960000</v>
+      </c>
+      <c r="J25" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="K25" s="28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I26" s="3">
+        <v>81920000</v>
+      </c>
+      <c r="J26" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="K26" s="29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{937DE6D2-C662-453A-A596-3DF68D92F3F8}">
+  <dimension ref="A1:Q28"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:O3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="12.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A1" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="P1" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="46" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>100</v>
+      </c>
+      <c r="B2" s="26">
+        <v>141</v>
+      </c>
+      <c r="C2" s="26">
+        <v>197</v>
+      </c>
+      <c r="D2" s="31">
+        <v>2014</v>
+      </c>
+      <c r="E2" s="31">
+        <v>2378</v>
+      </c>
+      <c r="F2" s="41">
+        <v>214</v>
+      </c>
+      <c r="G2" s="42">
+        <v>253</v>
+      </c>
+      <c r="H2" s="42">
+        <v>573</v>
+      </c>
+      <c r="J2" s="3">
+        <v>100</v>
+      </c>
+      <c r="K2" s="26">
+        <v>14.1</v>
+      </c>
+      <c r="L2" s="26">
+        <v>197</v>
+      </c>
+      <c r="M2" s="31">
+        <v>2014</v>
+      </c>
+      <c r="N2" s="31">
+        <v>2378</v>
+      </c>
+      <c r="O2" s="41">
+        <v>214</v>
+      </c>
+      <c r="P2" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q2" s="42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" s="3">
+        <v>200</v>
+      </c>
+      <c r="B3" s="27">
+        <v>327</v>
+      </c>
+      <c r="C3" s="27">
+        <v>1961</v>
+      </c>
+      <c r="D3" s="30">
+        <v>7999</v>
+      </c>
+      <c r="E3" s="30">
+        <v>14673</v>
+      </c>
+      <c r="F3" s="43">
+        <v>765</v>
+      </c>
+      <c r="G3" s="44">
+        <v>2433</v>
+      </c>
+      <c r="H3" s="44">
+        <v>6747</v>
+      </c>
+      <c r="J3" s="3">
+        <v>200</v>
+      </c>
+      <c r="K3" s="27">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="L3" s="27">
+        <v>1961</v>
+      </c>
+      <c r="M3" s="30">
+        <v>7999</v>
+      </c>
+      <c r="N3" s="30">
+        <v>14673</v>
+      </c>
+      <c r="O3" s="43">
+        <v>765</v>
+      </c>
+      <c r="P3" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q3" s="44" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
+        <v>400</v>
+      </c>
+      <c r="B4" s="27">
+        <v>682</v>
+      </c>
+      <c r="C4" s="27">
+        <v>9375</v>
+      </c>
+      <c r="D4" s="30">
+        <v>27867</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="43">
+        <v>3422</v>
+      </c>
+      <c r="G4" s="44">
+        <v>14679</v>
+      </c>
+      <c r="H4" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="J4" s="3">
+        <v>400</v>
+      </c>
+      <c r="K4" s="27">
+        <v>68.2</v>
+      </c>
+      <c r="L4" s="27">
+        <v>9375</v>
+      </c>
+      <c r="M4" s="30">
+        <v>27867</v>
+      </c>
+      <c r="N4" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="O4" s="43">
+        <v>3422</v>
+      </c>
+      <c r="P4" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q4" s="44" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" s="3">
+        <v>800</v>
+      </c>
+      <c r="B5" s="27">
+        <v>1605</v>
+      </c>
+      <c r="C5" s="27">
+        <v>44574</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="43">
+        <v>10416</v>
+      </c>
+      <c r="G5" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="3">
+        <v>800</v>
+      </c>
+      <c r="K5" s="27">
+        <v>160.5</v>
+      </c>
+      <c r="L5" s="27">
+        <v>44574</v>
+      </c>
+      <c r="M5" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="O5" s="43">
+        <v>10416</v>
+      </c>
+      <c r="P5" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" s="3">
+        <v>1600</v>
+      </c>
+      <c r="B6" s="27">
+        <v>3427</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="43">
+        <v>36358</v>
+      </c>
+      <c r="G6" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="3">
+        <v>1600</v>
+      </c>
+      <c r="K6" s="27">
+        <v>342.7</v>
+      </c>
+      <c r="L6" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="M6" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="N6" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="O6" s="43">
+        <v>36358</v>
+      </c>
+      <c r="P6" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" s="3">
+        <v>3200</v>
+      </c>
+      <c r="B7" s="27">
+        <v>6283</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="3">
+        <v>3200</v>
+      </c>
+      <c r="K7" s="27">
+        <v>628.29999999999995</v>
+      </c>
+      <c r="L7" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="M7" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="N7" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="O7" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
+        <v>6400</v>
+      </c>
+      <c r="B8" s="27">
+        <v>12287</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="3">
+        <v>6400</v>
+      </c>
+      <c r="K8" s="27">
+        <v>1228.7</v>
+      </c>
+      <c r="L8" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="N8" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="O8" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="P8" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" s="3">
+        <v>12800</v>
+      </c>
+      <c r="B9" s="27">
+        <v>27594</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="3">
+        <v>12800</v>
+      </c>
+      <c r="K9" s="27">
+        <v>2759.4</v>
+      </c>
+      <c r="L9" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="M9" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="N9" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="O9" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="P9" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10" s="3">
+        <v>25600</v>
+      </c>
+      <c r="B10" s="27">
+        <v>58229</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="3">
+        <v>25600</v>
+      </c>
+      <c r="K10" s="27">
+        <v>5822.9</v>
+      </c>
+      <c r="L10" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="M10" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="N10" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="O10" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="P10" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11" s="3">
+        <v>51200</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="3">
+        <v>51200</v>
+      </c>
+      <c r="K11" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="M11" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="N11" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="O11" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="P11" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="2">
+        <v>10000</v>
+      </c>
+      <c r="C13">
+        <v>1000</v>
+      </c>
+      <c r="D13">
+        <v>1000</v>
+      </c>
+      <c r="E13">
+        <v>1000</v>
+      </c>
+      <c r="F13" s="47">
+        <v>1000</v>
+      </c>
+      <c r="G13" s="47">
+        <v>10</v>
+      </c>
+      <c r="H13" s="47">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" s="24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="3">
+        <v>100</v>
+      </c>
+      <c r="B18" s="26">
+        <f>141/$B$13</f>
+        <v>1.41E-2</v>
+      </c>
+      <c r="C18" s="26">
+        <f>197/$C$13</f>
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="D18" s="27">
+        <f>B18/C18</f>
+        <v>7.1573604060913704E-2</v>
+      </c>
+      <c r="F18" s="3">
+        <v>100</v>
+      </c>
+      <c r="G18" s="31">
+        <v>2.0139999999999998</v>
+      </c>
+      <c r="H18" s="26">
+        <f>197/$C$13</f>
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="I18" s="27">
+        <f>G18/H18</f>
+        <v>10.223350253807105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="3">
+        <v>200</v>
+      </c>
+      <c r="B19" s="27">
+        <f>327/$B$13</f>
+        <v>3.27E-2</v>
+      </c>
+      <c r="C19" s="27">
+        <f>1961/$C$13</f>
+        <v>1.9610000000000001</v>
+      </c>
+      <c r="D19" s="27">
+        <f t="shared" ref="D19:D22" si="0">B19/C19</f>
+        <v>1.6675165731769505E-2</v>
+      </c>
+      <c r="F19" s="3">
+        <v>200</v>
+      </c>
+      <c r="G19" s="30">
+        <v>7.9989999999999997</v>
+      </c>
+      <c r="H19" s="27">
+        <f>1961/$C$13</f>
+        <v>1.9610000000000001</v>
+      </c>
+      <c r="I19" s="27">
+        <f t="shared" ref="I19:I20" si="1">G19/H19</f>
+        <v>4.0790413054563999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="3">
+        <v>400</v>
+      </c>
+      <c r="B20" s="27">
+        <f>682/$B$13</f>
+        <v>6.8199999999999997E-2</v>
+      </c>
+      <c r="C20" s="27">
+        <f>9375/$C$13</f>
+        <v>9.375</v>
+      </c>
+      <c r="D20" s="27">
+        <f t="shared" si="0"/>
+        <v>7.2746666666666663E-3</v>
+      </c>
+      <c r="F20" s="3">
+        <v>400</v>
+      </c>
+      <c r="G20" s="30">
+        <v>27.867000000000001</v>
+      </c>
+      <c r="H20" s="27">
+        <f>9375/$C$13</f>
+        <v>9.375</v>
+      </c>
+      <c r="I20" s="27">
+        <f t="shared" si="1"/>
+        <v>2.97248</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="3">
+        <v>800</v>
+      </c>
+      <c r="B21" s="27">
+        <f>1605/$B$13</f>
+        <v>0.1605</v>
+      </c>
+      <c r="C21" s="27">
+        <f>44574/$C$13</f>
+        <v>44.573999999999998</v>
+      </c>
+      <c r="D21" s="27">
+        <f t="shared" si="0"/>
+        <v>3.6007538026652311E-3</v>
+      </c>
+      <c r="F21" s="3">
+        <v>800</v>
+      </c>
+      <c r="G21" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21" s="27">
+        <f>44574/$C$13</f>
+        <v>44.573999999999998</v>
+      </c>
+      <c r="I21" s="27"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="3">
+        <v>1600</v>
+      </c>
+      <c r="B22" s="27">
+        <f>34257/$B$13</f>
+        <v>3.4257</v>
+      </c>
+      <c r="C22" s="27">
+        <f>164291/$C$13</f>
+        <v>164.291</v>
+      </c>
+      <c r="D22" s="27">
+        <f t="shared" si="0"/>
+        <v>2.085141608487379E-2</v>
+      </c>
+      <c r="F22" s="3">
+        <v>1600</v>
+      </c>
+      <c r="G22" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="H22" s="27">
+        <f>164291/$C$13</f>
+        <v>164.291</v>
+      </c>
+      <c r="I22" s="27"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="3">
+        <v>3200</v>
+      </c>
+      <c r="B23" s="27">
+        <v>6283</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="27"/>
+      <c r="F23" s="3">
+        <v>3200</v>
+      </c>
+      <c r="G23" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="H23" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="I23" s="27"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="3">
+        <v>6400</v>
+      </c>
+      <c r="B24" s="27">
+        <f>12287/$B$13</f>
+        <v>1.2286999999999999</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="27"/>
+      <c r="F24" s="3">
+        <v>6400</v>
+      </c>
+      <c r="G24" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="H24" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="I24" s="27"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" s="3">
+        <v>12800</v>
+      </c>
+      <c r="B25" s="27">
+        <f>27594/$B$13</f>
+        <v>2.7593999999999999</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="27"/>
+      <c r="F25" s="3">
+        <v>12800</v>
+      </c>
+      <c r="G25" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="I25" s="27"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="3">
+        <v>25600</v>
+      </c>
+      <c r="B26" s="27">
+        <f>58229/$B$13</f>
+        <v>5.8228999999999997</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="27"/>
+      <c r="F26" s="3">
+        <v>25600</v>
+      </c>
+      <c r="G26" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="H26" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="I26" s="27"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="3">
+        <v>51200</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="40"/>
+      <c r="F27" s="3">
+        <v>51200</v>
+      </c>
+      <c r="G27" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="I27" s="40"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C28" s="48"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E60BD896-48C5-4915-BDA1-8F872823DB6E}">
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="20.90625" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" customWidth="1"/>
+    <col min="8" max="8" width="21.6328125" customWidth="1"/>
+    <col min="9" max="9" width="18.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="51" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>200</v>
+      </c>
+      <c r="B2" s="27">
+        <v>74</v>
+      </c>
+      <c r="C2" s="27">
+        <v>239</v>
+      </c>
+      <c r="D2" s="2">
+        <v>131</v>
+      </c>
+      <c r="F2" s="3">
+        <v>200</v>
+      </c>
+      <c r="G2" s="49">
+        <v>7.4</v>
+      </c>
+      <c r="H2" s="49">
+        <v>2.39</v>
+      </c>
+      <c r="I2" s="49">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="J2" s="49">
+        <f>H2/G2</f>
+        <v>0.32297297297297295</v>
+      </c>
+      <c r="K2" s="49">
+        <f>I2/H2</f>
+        <v>5.4811715481171551E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="3">
+        <v>400</v>
+      </c>
+      <c r="B3" s="27">
+        <v>566</v>
+      </c>
+      <c r="C3" s="27">
+        <v>1704</v>
+      </c>
+      <c r="D3" s="2">
+        <v>797</v>
+      </c>
+      <c r="F3" s="3">
+        <v>400</v>
+      </c>
+      <c r="G3" s="49">
+        <v>56.6</v>
+      </c>
+      <c r="H3" s="49">
+        <v>17.04</v>
+      </c>
+      <c r="I3" s="49">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="J3" s="49">
+        <f t="shared" ref="J3:J7" si="0">H3/G3</f>
+        <v>0.30106007067137808</v>
+      </c>
+      <c r="K3" s="49">
+        <f t="shared" ref="K3:K5" si="1">I3/H3</f>
+        <v>4.6772300469483573E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
+        <v>800</v>
+      </c>
+      <c r="B4" s="27">
+        <v>4345</v>
+      </c>
+      <c r="C4" s="27">
+        <v>9901</v>
+      </c>
+      <c r="D4" s="2">
+        <v>4986</v>
+      </c>
+      <c r="F4" s="3">
+        <v>800</v>
+      </c>
+      <c r="G4" s="49">
+        <v>434.5</v>
+      </c>
+      <c r="H4" s="49">
+        <v>99.01</v>
+      </c>
+      <c r="I4" s="49">
+        <v>4.9859999999999998</v>
+      </c>
+      <c r="J4" s="49">
+        <f t="shared" si="0"/>
+        <v>0.22787111622554662</v>
+      </c>
+      <c r="K4" s="49">
+        <f t="shared" si="1"/>
+        <v>5.0358549641450354E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="3">
+        <v>1600</v>
+      </c>
+      <c r="B5" s="27">
+        <v>25092</v>
+      </c>
+      <c r="C5" s="27">
+        <v>62354</v>
+      </c>
+      <c r="D5" s="2">
+        <v>31987</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1600</v>
+      </c>
+      <c r="G5" s="49">
+        <v>2509.1999999999998</v>
+      </c>
+      <c r="H5" s="49">
+        <v>623.54</v>
+      </c>
+      <c r="I5" s="49">
+        <v>31.986999999999998</v>
+      </c>
+      <c r="J5" s="49">
+        <f t="shared" si="0"/>
+        <v>0.24850151442690899</v>
+      </c>
+      <c r="K5" s="49">
+        <f t="shared" si="1"/>
+        <v>5.1299034544696413E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
+        <v>3200</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="6">
+        <v>3200</v>
+      </c>
+      <c r="G6" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
+        <v>6400</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="6">
+        <v>6400</v>
+      </c>
+      <c r="G7" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>100</v>
+      </c>
+      <c r="D9">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>